<commit_message>
Update EU2 GPP 2023 Codebook.xlsx
</commit_message>
<xml_diff>
--- a/inputs/EU2 GPP 2023 Codebook.xlsx
+++ b/inputs/EU2 GPP 2023 Codebook.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ctoruno\Documents\GitHub\EU-copilot\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wjproject.sharepoint.com/research/Programmatic/EU Subnational/EU-S Data/GPP/0. Metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E30A9DF-7B1B-413C-BF0E-0CA537CA2DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1359" documentId="8_{65496F24-8EF0-4EA9-80D0-E64665E9412B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7602A446-90F5-464B-A190-08ADA5740174}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Naming System" sheetId="26" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Codebook!$A$1:$D$451</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Codebook!$A$1:$J$445</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3680" uniqueCount="1737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3698" uniqueCount="1744">
   <si>
     <t>Variable</t>
   </si>
@@ -5812,6 +5812,9 @@
     <t>EU_q13k</t>
   </si>
   <si>
+    <t>2023  EU Questionnaire</t>
+  </si>
+  <si>
     <t>EU_q14_1</t>
   </si>
   <si>
@@ -6091,9 +6094,6 @@
     <t>Problem Description</t>
   </si>
   <si>
-    <t>Pos</t>
-  </si>
-  <si>
     <t>Problem Resolution</t>
   </si>
   <si>
@@ -7780,7 +7780,30 @@
     <t>AJE_description_8</t>
   </si>
   <si>
-    <t>2023 EU Questionnaire</t>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>incpp</t>
+  </si>
+  <si>
+    <t>Is the aforementioned political party the incumbent political party?</t>
+  </si>
+  <si>
+    <t>Post-processing variable</t>
+  </si>
+  <si>
+    <t>Created by recoding voteintention and assigning 1 (Yes) to those who mentioned the incumbent political party and 2 (No) otherwise</t>
+  </si>
+  <si>
+    <t>ethni_groups</t>
+  </si>
+  <si>
+    <t>1=Main Ethnicity
+2=EU minor ethnicity
+3=Non-EU minor ethnicity</t>
+  </si>
+  <si>
+    <t>Created by recoding ethni into three different groups</t>
   </si>
 </sst>
 </file>
@@ -7909,7 +7932,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -7976,6 +7999,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8312,13 +8341,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J443"/>
+  <dimension ref="A1:K445"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C391" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomRight" activeCell="J398" sqref="J398"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8362,7 +8391,7 @@
         <v>1379</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>1736</v>
+        <v>1086</v>
       </c>
       <c r="J1" s="8" t="s">
         <v>1466</v>
@@ -8382,7 +8411,7 @@
         <v>1714</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>1027</v>
+        <v>1739</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>1699</v>
@@ -8443,7 +8472,7 @@
         <v>1714</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>1027</v>
+        <v>1739</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>1699</v>
@@ -8475,7 +8504,7 @@
         <v>1714</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>1027</v>
+        <v>1739</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>1699</v>
@@ -8507,7 +8536,7 @@
         <v>1714</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>1027</v>
+        <v>1739</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>1699</v>
@@ -8539,7 +8568,7 @@
         <v>1714</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>1027</v>
+        <v>1739</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>1699</v>
@@ -8571,7 +8600,7 @@
         <v>1714</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>1027</v>
+        <v>1739</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>1699</v>
@@ -8632,7 +8661,7 @@
         <v>1714</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>1027</v>
+        <v>1739</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>1699</v>
@@ -8664,7 +8693,7 @@
         <v>1714</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>1027</v>
+        <v>1739</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>1699</v>
@@ -10865,7 +10894,7 @@
         <v>1027</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="I93" s="3" t="s">
         <v>256</v>
@@ -10891,7 +10920,7 @@
         <v>1027</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="I94" s="3" t="s">
         <v>258</v>
@@ -10917,7 +10946,7 @@
         <v>1027</v>
       </c>
       <c r="H95" s="3" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="I95" s="3" t="s">
         <v>260</v>
@@ -10943,7 +10972,7 @@
         <v>1027</v>
       </c>
       <c r="H96" s="3" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="I96" s="3" t="s">
         <v>262</v>
@@ -10969,7 +10998,7 @@
         <v>1027</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="I97" s="3" t="s">
         <v>264</v>
@@ -10995,7 +11024,7 @@
         <v>1027</v>
       </c>
       <c r="H98" s="3" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="I98" s="3" t="s">
         <v>266</v>
@@ -11021,7 +11050,7 @@
         <v>1027</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="I99" s="3" t="s">
         <v>268</v>
@@ -11047,7 +11076,7 @@
         <v>1027</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="I100" s="3" t="s">
         <v>270</v>
@@ -11073,7 +11102,7 @@
         <v>1027</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="I101" s="3" t="s">
         <v>272</v>
@@ -11099,7 +11128,7 @@
         <v>1027</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="I102" s="3" t="s">
         <v>274</v>
@@ -11125,7 +11154,7 @@
         <v>1027</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="I103" s="3" t="s">
         <v>276</v>
@@ -11151,7 +11180,7 @@
         <v>1027</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="I104" s="3" t="s">
         <v>278</v>
@@ -11177,7 +11206,7 @@
         <v>1027</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="I105" s="3" t="s">
         <v>280</v>
@@ -11203,7 +11232,7 @@
         <v>1027</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="I106" s="3" t="s">
         <v>282</v>
@@ -11223,13 +11252,13 @@
         <v>991</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G107" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H107" s="3" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="I107" s="3" t="s">
         <v>284</v>
@@ -11249,13 +11278,13 @@
         <v>991</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G108" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H108" s="3" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="I108" s="3" t="s">
         <v>287</v>
@@ -11275,13 +11304,13 @@
         <v>991</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G109" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H109" s="3" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="I109" s="3" t="s">
         <v>289</v>
@@ -11301,13 +11330,13 @@
         <v>991</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G110" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H110" s="3" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="I110" s="3" t="s">
         <v>291</v>
@@ -11327,13 +11356,13 @@
         <v>991</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G111" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H111" s="3" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="I111" s="3" t="s">
         <v>293</v>
@@ -11353,13 +11382,13 @@
         <v>991</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G112" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H112" s="3" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="I112" s="3" t="s">
         <v>295</v>
@@ -11379,13 +11408,13 @@
         <v>991</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G113" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H113" s="3" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="I113" s="3" t="s">
         <v>297</v>
@@ -11405,13 +11434,13 @@
         <v>991</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G114" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H114" s="3" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="I114" s="3" t="s">
         <v>299</v>
@@ -11431,13 +11460,13 @@
         <v>991</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G115" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="I115" s="3" t="s">
         <v>301</v>
@@ -11457,13 +11486,13 @@
         <v>991</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G116" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H116" s="3" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="I116" s="3" t="s">
         <v>303</v>
@@ -11483,13 +11512,13 @@
         <v>991</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G117" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H117" s="3" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="I117" s="3" t="s">
         <v>305</v>
@@ -11509,13 +11538,13 @@
         <v>991</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G118" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H118" s="3" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="I118" s="3" t="s">
         <v>307</v>
@@ -11535,13 +11564,13 @@
         <v>991</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G119" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H119" s="3" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="I119" s="3" t="s">
         <v>309</v>
@@ -11561,13 +11590,13 @@
         <v>991</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G120" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H120" s="3" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="I120" s="3" t="s">
         <v>311</v>
@@ -11587,13 +11616,13 @@
         <v>991</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G121" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H121" s="3" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="I121" s="3" t="s">
         <v>313</v>
@@ -11613,13 +11642,13 @@
         <v>991</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G122" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H122" s="3" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="I122" s="3" t="s">
         <v>315</v>
@@ -11639,13 +11668,13 @@
         <v>991</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G123" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H123" s="3" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="I123" s="3" t="s">
         <v>317</v>
@@ -11665,13 +11694,13 @@
         <v>991</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G124" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H124" s="3" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="I124" s="3" t="s">
         <v>319</v>
@@ -11691,13 +11720,13 @@
         <v>991</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G125" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H125" s="3" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="I125" s="3" t="s">
         <v>321</v>
@@ -11717,13 +11746,13 @@
         <v>991</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G126" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H126" s="3" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="I126" s="3" t="s">
         <v>323</v>
@@ -11743,13 +11772,13 @@
         <v>991</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G127" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H127" s="3" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="I127" s="3" t="s">
         <v>325</v>
@@ -11769,13 +11798,13 @@
         <v>991</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G128" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H128" s="3" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="I128" s="3" t="s">
         <v>327</v>
@@ -11795,13 +11824,13 @@
         <v>991</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G129" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H129" s="3" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="I129" s="3" t="s">
         <v>329</v>
@@ -11821,13 +11850,13 @@
         <v>991</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G130" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H130" s="3" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="I130" s="3" t="s">
         <v>331</v>
@@ -11847,13 +11876,13 @@
         <v>991</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G131" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H131" s="3" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="I131" s="3" t="s">
         <v>333</v>
@@ -11873,13 +11902,13 @@
         <v>991</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G132" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H132" s="3" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="I132" s="3" t="s">
         <v>335</v>
@@ -11899,13 +11928,13 @@
         <v>991</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G133" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H133" s="3" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="I133" s="3" t="s">
         <v>337</v>
@@ -11925,13 +11954,13 @@
         <v>991</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G134" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H134" s="3" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="I134" s="3" t="s">
         <v>339</v>
@@ -11951,13 +11980,13 @@
         <v>991</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G135" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H135" s="3" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="I135" s="3" t="s">
         <v>341</v>
@@ -11977,13 +12006,13 @@
         <v>991</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G136" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H136" s="3" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="I136" s="3" t="s">
         <v>343</v>
@@ -12003,13 +12032,13 @@
         <v>991</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G137" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H137" s="3" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="I137" s="3" t="s">
         <v>345</v>
@@ -12029,13 +12058,13 @@
         <v>991</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G138" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H138" s="3" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="I138" s="3" t="s">
         <v>347</v>
@@ -12055,13 +12084,13 @@
         <v>991</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G139" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H139" s="3" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="I139" s="3" t="s">
         <v>349</v>
@@ -12081,13 +12110,13 @@
         <v>991</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G140" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H140" s="3" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="I140" s="3" t="s">
         <v>351</v>
@@ -12107,13 +12136,13 @@
         <v>991</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G141" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H141" s="3" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="I141" s="3" t="s">
         <v>353</v>
@@ -12133,13 +12162,13 @@
         <v>991</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G142" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H142" s="3" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="I142" s="3" t="s">
         <v>355</v>
@@ -12159,13 +12188,13 @@
         <v>991</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G143" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H143" s="3" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="I143" s="3" t="s">
         <v>357</v>
@@ -12185,13 +12214,13 @@
         <v>991</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G144" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H144" s="3" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="I144" s="3" t="s">
         <v>359</v>
@@ -12211,13 +12240,13 @@
         <v>991</v>
       </c>
       <c r="F145" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G145" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H145" s="3" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="I145" s="3" t="s">
         <v>361</v>
@@ -12237,13 +12266,13 @@
         <v>991</v>
       </c>
       <c r="F146" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G146" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H146" s="3" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="I146" s="3" t="s">
         <v>364</v>
@@ -12263,13 +12292,13 @@
         <v>991</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G147" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H147" s="3" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="I147" s="3" t="s">
         <v>366</v>
@@ -12289,13 +12318,13 @@
         <v>991</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G148" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H148" s="3" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="I148" s="3" t="s">
         <v>368</v>
@@ -12315,13 +12344,13 @@
         <v>991</v>
       </c>
       <c r="F149" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G149" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H149" s="3" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="I149" s="3" t="s">
         <v>370</v>
@@ -12341,13 +12370,13 @@
         <v>991</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G150" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H150" s="3" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="I150" s="3" t="s">
         <v>372</v>
@@ -12367,13 +12396,13 @@
         <v>991</v>
       </c>
       <c r="F151" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G151" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H151" s="3" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="I151" s="3" t="s">
         <v>374</v>
@@ -12393,13 +12422,13 @@
         <v>991</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G152" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H152" s="3" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="I152" s="3" t="s">
         <v>376</v>
@@ -12419,13 +12448,13 @@
         <v>991</v>
       </c>
       <c r="F153" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G153" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H153" s="3" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="I153" s="3" t="s">
         <v>378</v>
@@ -12445,13 +12474,13 @@
         <v>991</v>
       </c>
       <c r="F154" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G154" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H154" s="3" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="I154" s="3" t="s">
         <v>380</v>
@@ -12471,13 +12500,13 @@
         <v>991</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G155" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H155" s="3" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="I155" s="3" t="s">
         <v>382</v>
@@ -12497,13 +12526,13 @@
         <v>991</v>
       </c>
       <c r="F156" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G156" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H156" s="3" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="I156" s="3" t="s">
         <v>384</v>
@@ -12523,13 +12552,13 @@
         <v>991</v>
       </c>
       <c r="F157" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G157" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H157" s="3" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="I157" s="3" t="s">
         <v>386</v>
@@ -12549,13 +12578,13 @@
         <v>991</v>
       </c>
       <c r="F158" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G158" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H158" s="3" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="I158" s="3" t="s">
         <v>388</v>
@@ -12575,13 +12604,13 @@
         <v>991</v>
       </c>
       <c r="F159" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G159" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H159" s="3" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="I159" s="3" t="s">
         <v>390</v>
@@ -12601,13 +12630,13 @@
         <v>991</v>
       </c>
       <c r="F160" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G160" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H160" s="3" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="I160" s="3" t="s">
         <v>392</v>
@@ -12627,13 +12656,13 @@
         <v>991</v>
       </c>
       <c r="F161" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G161" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H161" s="3" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="I161" s="3" t="s">
         <v>394</v>
@@ -12653,13 +12682,13 @@
         <v>991</v>
       </c>
       <c r="F162" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G162" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H162" s="3" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="I162" s="3" t="s">
         <v>396</v>
@@ -12679,13 +12708,13 @@
         <v>991</v>
       </c>
       <c r="F163" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G163" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H163" s="3" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="I163" s="3" t="s">
         <v>398</v>
@@ -12705,13 +12734,13 @@
         <v>991</v>
       </c>
       <c r="F164" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G164" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H164" s="3" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="I164" s="3" t="s">
         <v>400</v>
@@ -12731,13 +12760,13 @@
         <v>991</v>
       </c>
       <c r="F165" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G165" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H165" s="3" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="I165" s="3" t="s">
         <v>402</v>
@@ -12757,13 +12786,13 @@
         <v>991</v>
       </c>
       <c r="F166" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G166" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H166" s="3" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="I166" s="3" t="s">
         <v>404</v>
@@ -12783,13 +12812,13 @@
         <v>991</v>
       </c>
       <c r="F167" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G167" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H167" s="3" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="I167" s="3" t="s">
         <v>406</v>
@@ -12809,13 +12838,13 @@
         <v>991</v>
       </c>
       <c r="F168" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G168" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H168" s="3" t="s">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="I168" s="3" t="s">
         <v>408</v>
@@ -12835,13 +12864,13 @@
         <v>991</v>
       </c>
       <c r="F169" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G169" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H169" s="3" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="I169" s="3" t="s">
         <v>410</v>
@@ -12861,13 +12890,13 @@
         <v>991</v>
       </c>
       <c r="F170" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G170" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H170" s="3" t="s">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="I170" s="3" t="s">
         <v>412</v>
@@ -12887,13 +12916,13 @@
         <v>991</v>
       </c>
       <c r="F171" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G171" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H171" s="3" t="s">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="I171" s="3" t="s">
         <v>414</v>
@@ -12913,13 +12942,13 @@
         <v>991</v>
       </c>
       <c r="F172" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G172" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H172" s="3" t="s">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="I172" s="3" t="s">
         <v>416</v>
@@ -12939,13 +12968,13 @@
         <v>991</v>
       </c>
       <c r="F173" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G173" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H173" s="3" t="s">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="I173" s="3" t="s">
         <v>418</v>
@@ -12965,13 +12994,13 @@
         <v>991</v>
       </c>
       <c r="F174" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G174" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H174" s="3" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="I174" s="3" t="s">
         <v>420</v>
@@ -12991,13 +13020,13 @@
         <v>991</v>
       </c>
       <c r="F175" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G175" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H175" s="3" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="I175" s="3" t="s">
         <v>422</v>
@@ -13017,13 +13046,13 @@
         <v>991</v>
       </c>
       <c r="F176" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G176" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H176" s="3" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="I176" s="3" t="s">
         <v>424</v>
@@ -13043,13 +13072,13 @@
         <v>991</v>
       </c>
       <c r="F177" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G177" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H177" s="3" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="I177" s="3" t="s">
         <v>426</v>
@@ -13069,13 +13098,13 @@
         <v>991</v>
       </c>
       <c r="F178" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G178" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H178" s="3" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="I178" s="3" t="s">
         <v>428</v>
@@ -13095,13 +13124,13 @@
         <v>991</v>
       </c>
       <c r="F179" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G179" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H179" s="3" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="I179" s="3" t="s">
         <v>430</v>
@@ -13121,13 +13150,13 @@
         <v>991</v>
       </c>
       <c r="F180" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G180" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H180" s="3" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="I180" s="3" t="s">
         <v>432</v>
@@ -13147,13 +13176,13 @@
         <v>991</v>
       </c>
       <c r="F181" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G181" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H181" s="3" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="I181" s="3" t="s">
         <v>434</v>
@@ -13173,13 +13202,13 @@
         <v>991</v>
       </c>
       <c r="F182" s="3" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="G182" s="3" t="s">
         <v>1027</v>
       </c>
       <c r="H182" s="3" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="I182" s="3" t="s">
         <v>436</v>
@@ -13199,13 +13228,13 @@
         <v>991</v>
       </c>
       <c r="F183" s="3" t="s">
+        <v>1178</v>
+      </c>
+      <c r="G183" s="3" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H183" s="3" t="s">
         <v>1177</v>
-      </c>
-      <c r="G183" s="3" t="s">
-        <v>1027</v>
-      </c>
-      <c r="H183" s="3" t="s">
-        <v>1176</v>
       </c>
       <c r="I183" s="3" t="s">
         <v>438</v>
@@ -13225,7 +13254,7 @@
         <v>991</v>
       </c>
       <c r="F184" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="G184" s="3" t="s">
         <v>1027</v>
@@ -13251,7 +13280,7 @@
         <v>991</v>
       </c>
       <c r="F185" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="G185" s="3" t="s">
         <v>1027</v>
@@ -13277,7 +13306,7 @@
         <v>991</v>
       </c>
       <c r="F186" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="G186" s="3" t="s">
         <v>1027</v>
@@ -13303,7 +13332,7 @@
         <v>991</v>
       </c>
       <c r="F187" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="G187" s="3" t="s">
         <v>1027</v>
@@ -13329,7 +13358,7 @@
         <v>991</v>
       </c>
       <c r="F188" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="G188" s="3" t="s">
         <v>1027</v>
@@ -13355,7 +13384,7 @@
         <v>991</v>
       </c>
       <c r="F189" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="G189" s="3" t="s">
         <v>1027</v>
@@ -13381,7 +13410,7 @@
         <v>991</v>
       </c>
       <c r="F190" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="G190" s="3" t="s">
         <v>1027</v>
@@ -13407,7 +13436,7 @@
         <v>991</v>
       </c>
       <c r="F191" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="G191" s="3" t="s">
         <v>1027</v>
@@ -13433,7 +13462,7 @@
         <v>991</v>
       </c>
       <c r="F192" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="G192" s="3" t="s">
         <v>1027</v>
@@ -13459,7 +13488,7 @@
         <v>991</v>
       </c>
       <c r="F193" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="G193" s="3" t="s">
         <v>1027</v>
@@ -13485,7 +13514,7 @@
         <v>991</v>
       </c>
       <c r="F194" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="G194" s="3" t="s">
         <v>1027</v>
@@ -13511,7 +13540,7 @@
         <v>991</v>
       </c>
       <c r="F195" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="G195" s="3" t="s">
         <v>1027</v>
@@ -13537,7 +13566,7 @@
         <v>991</v>
       </c>
       <c r="F196" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="G196" s="3" t="s">
         <v>1027</v>
@@ -13563,7 +13592,7 @@
         <v>991</v>
       </c>
       <c r="F197" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="G197" s="3" t="s">
         <v>1027</v>
@@ -13589,7 +13618,7 @@
         <v>991</v>
       </c>
       <c r="F198" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="G198" s="3" t="s">
         <v>1027</v>
@@ -13615,7 +13644,7 @@
         <v>991</v>
       </c>
       <c r="F199" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="G199" s="3" t="s">
         <v>1027</v>
@@ -13641,7 +13670,7 @@
         <v>991</v>
       </c>
       <c r="F200" s="3" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="G200" s="3" t="s">
         <v>1027</v>
@@ -18836,18 +18865,18 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="397" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A397" s="3" t="s">
-        <v>858</v>
+        <v>1741</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="D397" s="3" t="s">
-        <v>860</v>
-      </c>
-      <c r="E397" s="3" t="s">
-        <v>1676</v>
+        <v>1742</v>
+      </c>
+      <c r="E397" s="9" t="s">
+        <v>1739</v>
       </c>
       <c r="F397" s="3" t="s">
         <v>1676</v>
@@ -18855,22 +18884,25 @@
       <c r="G397" s="3" t="s">
         <v>1027</v>
       </c>
-      <c r="H397" s="3" t="s">
+      <c r="H397" s="16" t="s">
+        <v>1451</v>
+      </c>
+      <c r="I397" s="16" t="s">
+        <v>1452</v>
+      </c>
+      <c r="J397" s="13" t="s">
+        <v>1743</v>
+      </c>
+    </row>
+    <row r="398" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A398" s="3" t="s">
         <v>858</v>
       </c>
-      <c r="I397" s="3" t="s">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="398" spans="1:10" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="A398" s="3" t="s">
-        <v>861</v>
-      </c>
       <c r="B398" s="3" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="D398" s="3" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="E398" s="3" t="s">
         <v>1676</v>
@@ -18882,21 +18914,21 @@
         <v>1027</v>
       </c>
       <c r="H398" s="3" t="s">
+        <v>858</v>
+      </c>
+      <c r="I398" s="3" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="399" spans="1:10" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="A399" s="3" t="s">
         <v>861</v>
       </c>
-      <c r="I398" s="3" t="s">
-        <v>861</v>
-      </c>
-    </row>
-    <row r="399" spans="1:10" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A399" s="3" t="s">
-        <v>864</v>
-      </c>
       <c r="B399" s="3" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="D399" s="3" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="E399" s="3" t="s">
         <v>1676</v>
@@ -18908,21 +18940,21 @@
         <v>1027</v>
       </c>
       <c r="H399" s="3" t="s">
+        <v>861</v>
+      </c>
+      <c r="I399" s="3" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="400" spans="1:10" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A400" s="3" t="s">
         <v>864</v>
       </c>
-      <c r="I399" s="3" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="400" spans="1:10" ht="153" x14ac:dyDescent="0.2">
-      <c r="A400" s="3" t="s">
-        <v>867</v>
-      </c>
       <c r="B400" s="3" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="D400" s="3" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="E400" s="3" t="s">
         <v>1676</v>
@@ -18934,21 +18966,21 @@
         <v>1027</v>
       </c>
       <c r="H400" s="3" t="s">
+        <v>864</v>
+      </c>
+      <c r="I400" s="3" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="401" spans="1:11" ht="153" x14ac:dyDescent="0.2">
+      <c r="A401" s="3" t="s">
         <v>867</v>
       </c>
-      <c r="I400" s="3" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="401" spans="1:9" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="A401" s="3" t="s">
-        <v>870</v>
-      </c>
       <c r="B401" s="3" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="D401" s="3" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="E401" s="3" t="s">
         <v>1676</v>
@@ -18960,23 +18992,23 @@
         <v>1027</v>
       </c>
       <c r="H401" s="3" t="s">
+        <v>867</v>
+      </c>
+      <c r="I401" s="3" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="402" spans="1:11" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A402" s="3" t="s">
         <v>870</v>
       </c>
-      <c r="I401" s="3" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="402" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A402" s="3" t="s">
-        <v>873</v>
-      </c>
       <c r="B402" s="3" t="s">
-        <v>874</v>
-      </c>
-      <c r="D402" s="10" t="s">
-        <v>875</v>
-      </c>
-      <c r="E402" s="17" t="s">
+        <v>871</v>
+      </c>
+      <c r="D402" s="3" t="s">
+        <v>872</v>
+      </c>
+      <c r="E402" s="3" t="s">
         <v>1676</v>
       </c>
       <c r="F402" s="3" t="s">
@@ -18986,23 +19018,23 @@
         <v>1027</v>
       </c>
       <c r="H402" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="I402" s="3" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="403" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="A403" s="3" t="s">
         <v>873</v>
       </c>
-      <c r="I402" s="3" t="s">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="403" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A403" s="3" t="s">
-        <v>876</v>
-      </c>
       <c r="B403" s="3" t="s">
-        <v>877</v>
-      </c>
-      <c r="D403" s="3" t="s">
-        <v>878</v>
-      </c>
-      <c r="E403" s="3" t="s">
+        <v>874</v>
+      </c>
+      <c r="D403" s="10" t="s">
+        <v>875</v>
+      </c>
+      <c r="E403" s="17" t="s">
         <v>1676</v>
       </c>
       <c r="F403" s="3" t="s">
@@ -19012,21 +19044,21 @@
         <v>1027</v>
       </c>
       <c r="H403" s="3" t="s">
+        <v>873</v>
+      </c>
+      <c r="I403" s="3" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="404" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+      <c r="A404" s="3" t="s">
         <v>876</v>
       </c>
-      <c r="I403" s="3" t="s">
-        <v>876</v>
-      </c>
-    </row>
-    <row r="404" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A404" s="3" t="s">
-        <v>879</v>
-      </c>
       <c r="B404" s="3" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="D404" s="3" t="s">
-        <v>230</v>
+        <v>878</v>
       </c>
       <c r="E404" s="3" t="s">
         <v>1676</v>
@@ -19038,21 +19070,21 @@
         <v>1027</v>
       </c>
       <c r="H404" s="3" t="s">
+        <v>876</v>
+      </c>
+      <c r="I404" s="3" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="405" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="A405" s="3" t="s">
         <v>879</v>
       </c>
-      <c r="I404" s="3" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="405" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A405" s="3" t="s">
-        <v>881</v>
-      </c>
       <c r="B405" s="3" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="D405" s="3" t="s">
-        <v>883</v>
+        <v>230</v>
       </c>
       <c r="E405" s="3" t="s">
         <v>1676</v>
@@ -19064,21 +19096,21 @@
         <v>1027</v>
       </c>
       <c r="H405" s="3" t="s">
+        <v>879</v>
+      </c>
+      <c r="I405" s="3" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="406" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="A406" s="3" t="s">
         <v>881</v>
       </c>
-      <c r="I405" s="3" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="406" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A406" s="3" t="s">
-        <v>884</v>
-      </c>
       <c r="B406" s="3" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
       <c r="D406" s="3" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
       <c r="E406" s="3" t="s">
         <v>1676</v>
@@ -19090,21 +19122,21 @@
         <v>1027</v>
       </c>
       <c r="H406" s="3" t="s">
+        <v>881</v>
+      </c>
+      <c r="I406" s="3" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="407" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A407" s="3" t="s">
         <v>884</v>
       </c>
-      <c r="I406" s="3" t="s">
-        <v>884</v>
-      </c>
-    </row>
-    <row r="407" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A407" s="2" t="s">
-        <v>887</v>
-      </c>
       <c r="B407" s="3" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
       <c r="D407" s="3" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="E407" s="3" t="s">
         <v>1676</v>
@@ -19115,22 +19147,22 @@
       <c r="G407" s="3" t="s">
         <v>1027</v>
       </c>
-      <c r="H407" s="19" t="s">
+      <c r="H407" s="3" t="s">
+        <v>884</v>
+      </c>
+      <c r="I407" s="3" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="408" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A408" s="2" t="s">
         <v>887</v>
       </c>
-      <c r="I407" s="2" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="408" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A408" s="3" t="s">
-        <v>1685</v>
-      </c>
       <c r="B408" s="3" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="D408" s="3" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
       <c r="E408" s="3" t="s">
         <v>1676</v>
@@ -19141,19 +19173,21 @@
       <c r="G408" s="3" t="s">
         <v>1027</v>
       </c>
-      <c r="H408" s="3" t="s">
-        <v>1681</v>
-      </c>
-      <c r="I408" s="3" t="s">
-        <v>890</v>
-      </c>
-    </row>
-    <row r="409" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="H408" s="19" t="s">
+        <v>887</v>
+      </c>
+      <c r="I408" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="J408" s="23"/>
+      <c r="K408" s="24"/>
+    </row>
+    <row r="409" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A409" s="3" t="s">
-        <v>1682</v>
+        <v>1685</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="D409" s="3" t="s">
         <v>892</v>
@@ -19168,21 +19202,23 @@
         <v>1027</v>
       </c>
       <c r="H409" s="3" t="s">
-        <v>1683</v>
+        <v>1681</v>
       </c>
       <c r="I409" s="3" t="s">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="410" spans="1:9" x14ac:dyDescent="0.2">
+        <v>890</v>
+      </c>
+      <c r="J409" s="23"/>
+      <c r="K409" s="23"/>
+    </row>
+    <row r="410" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A410" s="3" t="s">
-        <v>895</v>
+        <v>1682</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="D410" s="3" t="s">
-        <v>19</v>
+        <v>892</v>
       </c>
       <c r="E410" s="3" t="s">
         <v>1676</v>
@@ -19194,24 +19230,24 @@
         <v>1027</v>
       </c>
       <c r="H410" s="3" t="s">
-        <v>895</v>
+        <v>1683</v>
       </c>
       <c r="I410" s="3" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="411" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="411" spans="1:11" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A411" s="3" t="s">
-        <v>897</v>
-      </c>
-      <c r="B411" s="4" t="s">
-        <v>898</v>
+        <v>1737</v>
+      </c>
+      <c r="B411" s="3" t="s">
+        <v>1738</v>
       </c>
       <c r="D411" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="E411" s="3" t="s">
-        <v>1676</v>
+        <v>558</v>
+      </c>
+      <c r="E411" s="9" t="s">
+        <v>1739</v>
       </c>
       <c r="F411" s="3" t="s">
         <v>1676</v>
@@ -19219,22 +19255,25 @@
       <c r="G411" s="3" t="s">
         <v>1027</v>
       </c>
-      <c r="H411" s="3" t="s">
-        <v>899</v>
-      </c>
-      <c r="I411" s="3" t="s">
-        <v>897</v>
-      </c>
-    </row>
-    <row r="412" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="H411" s="16" t="s">
+        <v>1451</v>
+      </c>
+      <c r="I411" s="16" t="s">
+        <v>1452</v>
+      </c>
+      <c r="J411" s="13" t="s">
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="412" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A412" s="3" t="s">
-        <v>899</v>
+        <v>895</v>
       </c>
       <c r="B412" s="3" t="s">
-        <v>900</v>
+        <v>896</v>
       </c>
       <c r="D412" s="3" t="s">
-        <v>901</v>
+        <v>19</v>
       </c>
       <c r="E412" s="3" t="s">
         <v>1676</v>
@@ -19246,18 +19285,18 @@
         <v>1027</v>
       </c>
       <c r="H412" s="3" t="s">
-        <v>902</v>
+        <v>895</v>
       </c>
       <c r="I412" s="3" t="s">
-        <v>899</v>
-      </c>
-    </row>
-    <row r="413" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="413" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A413" s="3" t="s">
-        <v>902</v>
-      </c>
-      <c r="B413" s="3" t="s">
-        <v>903</v>
+        <v>897</v>
+      </c>
+      <c r="B413" s="4" t="s">
+        <v>898</v>
       </c>
       <c r="D413" s="3" t="s">
         <v>230</v>
@@ -19272,21 +19311,21 @@
         <v>1027</v>
       </c>
       <c r="H413" s="3" t="s">
-        <v>1686</v>
+        <v>899</v>
       </c>
       <c r="I413" s="3" t="s">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="414" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="414" spans="1:11" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A414" s="3" t="s">
-        <v>904</v>
+        <v>899</v>
       </c>
       <c r="B414" s="3" t="s">
-        <v>905</v>
+        <v>900</v>
       </c>
       <c r="D414" s="3" t="s">
-        <v>230</v>
+        <v>901</v>
       </c>
       <c r="E414" s="3" t="s">
         <v>1676</v>
@@ -19298,18 +19337,18 @@
         <v>1027</v>
       </c>
       <c r="H414" s="3" t="s">
-        <v>1687</v>
+        <v>902</v>
       </c>
       <c r="I414" s="3" t="s">
-        <v>904</v>
-      </c>
-    </row>
-    <row r="415" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="415" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A415" s="3" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>907</v>
+        <v>903</v>
       </c>
       <c r="D415" s="3" t="s">
         <v>230</v>
@@ -19324,21 +19363,21 @@
         <v>1027</v>
       </c>
       <c r="H415" s="3" t="s">
-        <v>1688</v>
+        <v>1686</v>
       </c>
       <c r="I415" s="3" t="s">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="416" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A416" s="2" t="s">
-        <v>908</v>
+        <v>902</v>
+      </c>
+    </row>
+    <row r="416" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="A416" s="3" t="s">
+        <v>904</v>
       </c>
       <c r="B416" s="3" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="D416" s="3" t="s">
-        <v>910</v>
+        <v>230</v>
       </c>
       <c r="E416" s="3" t="s">
         <v>1676</v>
@@ -19350,21 +19389,21 @@
         <v>1027</v>
       </c>
       <c r="H416" s="3" t="s">
-        <v>1689</v>
-      </c>
-      <c r="I416" s="2" t="s">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="417" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A417" s="2" t="s">
-        <v>911</v>
+        <v>1687</v>
+      </c>
+      <c r="I416" s="3" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="417" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A417" s="3" t="s">
+        <v>906</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>912</v>
+        <v>907</v>
       </c>
       <c r="D417" s="3" t="s">
-        <v>913</v>
+        <v>230</v>
       </c>
       <c r="E417" s="3" t="s">
         <v>1676</v>
@@ -19376,21 +19415,21 @@
         <v>1027</v>
       </c>
       <c r="H417" s="3" t="s">
-        <v>1690</v>
-      </c>
-      <c r="I417" s="2" t="s">
-        <v>911</v>
+        <v>1688</v>
+      </c>
+      <c r="I417" s="3" t="s">
+        <v>906</v>
       </c>
     </row>
     <row r="418" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A418" s="3" t="s">
-        <v>914</v>
+      <c r="A418" s="2" t="s">
+        <v>908</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>915</v>
+        <v>909</v>
       </c>
       <c r="D418" s="3" t="s">
-        <v>230</v>
+        <v>910</v>
       </c>
       <c r="E418" s="3" t="s">
         <v>1676</v>
@@ -19402,21 +19441,21 @@
         <v>1027</v>
       </c>
       <c r="H418" s="3" t="s">
-        <v>1691</v>
-      </c>
-      <c r="I418" s="3" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="419" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A419" s="3" t="s">
-        <v>916</v>
+        <v>1689</v>
+      </c>
+      <c r="I418" s="2" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="419" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A419" s="2" t="s">
+        <v>911</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>917</v>
+        <v>912</v>
       </c>
       <c r="D419" s="3" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="E419" s="3" t="s">
         <v>1676</v>
@@ -19428,21 +19467,21 @@
         <v>1027</v>
       </c>
       <c r="H419" s="3" t="s">
-        <v>1692</v>
-      </c>
-      <c r="I419" s="3" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="420" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A420" s="2" t="s">
-        <v>1694</v>
+        <v>1690</v>
+      </c>
+      <c r="I419" s="2" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="420" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A420" s="3" t="s">
+        <v>914</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>920</v>
+        <v>915</v>
       </c>
       <c r="D420" s="3" t="s">
-        <v>8</v>
+        <v>230</v>
       </c>
       <c r="E420" s="3" t="s">
         <v>1676</v>
@@ -19453,72 +19492,74 @@
       <c r="G420" s="3" t="s">
         <v>1027</v>
       </c>
-      <c r="H420" s="19" t="s">
+      <c r="H420" s="3" t="s">
+        <v>1691</v>
+      </c>
+      <c r="I420" s="3" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="421" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A421" s="3" t="s">
+        <v>916</v>
+      </c>
+      <c r="B421" s="3" t="s">
+        <v>917</v>
+      </c>
+      <c r="D421" s="3" t="s">
+        <v>918</v>
+      </c>
+      <c r="E421" s="3" t="s">
+        <v>1676</v>
+      </c>
+      <c r="F421" s="3" t="s">
+        <v>1676</v>
+      </c>
+      <c r="G421" s="3" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H421" s="3" t="s">
+        <v>1692</v>
+      </c>
+      <c r="I421" s="3" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="422" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A422" s="2" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B422" s="3" t="s">
+        <v>920</v>
+      </c>
+      <c r="D422" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E422" s="3" t="s">
+        <v>1676</v>
+      </c>
+      <c r="F422" s="3" t="s">
+        <v>1676</v>
+      </c>
+      <c r="G422" s="3" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H422" s="19" t="s">
         <v>919</v>
       </c>
-      <c r="I420" s="2" t="s">
+      <c r="I422" s="2" t="s">
         <v>919</v>
-      </c>
-    </row>
-    <row r="421" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A421" s="3" t="s">
-        <v>921</v>
-      </c>
-      <c r="B421" s="3" t="s">
-        <v>922</v>
-      </c>
-      <c r="D421" s="10"/>
-      <c r="E421" s="10" t="s">
-        <v>1677</v>
-      </c>
-      <c r="F421" s="18" t="s">
-        <v>1677</v>
-      </c>
-      <c r="G421" s="3" t="s">
-        <v>1027</v>
-      </c>
-      <c r="H421" s="3" t="s">
-        <v>921</v>
-      </c>
-      <c r="I421" s="3" t="s">
-        <v>921</v>
-      </c>
-    </row>
-    <row r="422" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A422" s="3" t="s">
-        <v>923</v>
-      </c>
-      <c r="B422" s="3" t="s">
-        <v>924</v>
-      </c>
-      <c r="D422" s="10"/>
-      <c r="E422" s="10" t="s">
-        <v>1677</v>
-      </c>
-      <c r="F422" s="18" t="s">
-        <v>1677</v>
-      </c>
-      <c r="G422" s="3" t="s">
-        <v>1027</v>
-      </c>
-      <c r="H422" s="3" t="s">
-        <v>923</v>
-      </c>
-      <c r="I422" s="3" t="s">
-        <v>923</v>
       </c>
     </row>
     <row r="423" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A423" s="3" t="s">
-        <v>1680</v>
+        <v>921</v>
       </c>
       <c r="B423" s="3" t="s">
-        <v>926</v>
-      </c>
-      <c r="D423" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E423" s="18" t="s">
+        <v>922</v>
+      </c>
+      <c r="D423" s="10"/>
+      <c r="E423" s="10" t="s">
         <v>1677</v>
       </c>
       <c r="F423" s="18" t="s">
@@ -19528,23 +19569,21 @@
         <v>1027</v>
       </c>
       <c r="H423" s="3" t="s">
-        <v>925</v>
+        <v>921</v>
       </c>
       <c r="I423" s="3" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="424" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="424" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A424" s="3" t="s">
-        <v>1679</v>
+        <v>923</v>
       </c>
       <c r="B424" s="3" t="s">
-        <v>928</v>
-      </c>
-      <c r="D424" s="3" t="s">
-        <v>929</v>
-      </c>
-      <c r="E424" s="18" t="s">
+        <v>924</v>
+      </c>
+      <c r="D424" s="10"/>
+      <c r="E424" s="10" t="s">
         <v>1677</v>
       </c>
       <c r="F424" s="18" t="s">
@@ -19554,21 +19593,21 @@
         <v>1027</v>
       </c>
       <c r="H424" s="3" t="s">
-        <v>1679</v>
+        <v>923</v>
       </c>
       <c r="I424" s="3" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="425" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="425" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A425" s="3" t="s">
-        <v>1695</v>
+        <v>1680</v>
       </c>
       <c r="B425" s="3" t="s">
-        <v>931</v>
+        <v>926</v>
       </c>
       <c r="D425" s="3" t="s">
-        <v>932</v>
+        <v>8</v>
       </c>
       <c r="E425" s="18" t="s">
         <v>1677</v>
@@ -19580,21 +19619,21 @@
         <v>1027</v>
       </c>
       <c r="H425" s="3" t="s">
-        <v>1678</v>
+        <v>925</v>
       </c>
       <c r="I425" s="3" t="s">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="426" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="426" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A426" s="3" t="s">
-        <v>1693</v>
+        <v>1679</v>
       </c>
       <c r="B426" s="3" t="s">
-        <v>934</v>
+        <v>928</v>
       </c>
       <c r="D426" s="3" t="s">
-        <v>935</v>
+        <v>929</v>
       </c>
       <c r="E426" s="18" t="s">
         <v>1677</v>
@@ -19606,21 +19645,21 @@
         <v>1027</v>
       </c>
       <c r="H426" s="3" t="s">
-        <v>933</v>
+        <v>1679</v>
       </c>
       <c r="I426" s="3" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="427" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="427" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A427" s="3" t="s">
-        <v>936</v>
-      </c>
-      <c r="B427" s="4" t="s">
-        <v>937</v>
+        <v>1695</v>
+      </c>
+      <c r="B427" s="3" t="s">
+        <v>931</v>
       </c>
       <c r="D427" s="3" t="s">
-        <v>938</v>
+        <v>932</v>
       </c>
       <c r="E427" s="18" t="s">
         <v>1677</v>
@@ -19632,21 +19671,21 @@
         <v>1027</v>
       </c>
       <c r="H427" s="3" t="s">
-        <v>936</v>
+        <v>1678</v>
       </c>
       <c r="I427" s="3" t="s">
-        <v>936</v>
+        <v>930</v>
       </c>
     </row>
     <row r="428" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A428" s="3" t="s">
-        <v>939</v>
+        <v>1693</v>
       </c>
       <c r="B428" s="3" t="s">
-        <v>940</v>
+        <v>934</v>
       </c>
       <c r="D428" s="3" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="E428" s="18" t="s">
         <v>1677</v>
@@ -19658,21 +19697,21 @@
         <v>1027</v>
       </c>
       <c r="H428" s="3" t="s">
-        <v>939</v>
+        <v>933</v>
       </c>
       <c r="I428" s="3" t="s">
-        <v>939</v>
+        <v>933</v>
       </c>
     </row>
     <row r="429" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A429" s="3" t="s">
-        <v>942</v>
-      </c>
-      <c r="B429" s="3" t="s">
-        <v>943</v>
+        <v>936</v>
+      </c>
+      <c r="B429" s="4" t="s">
+        <v>937</v>
       </c>
       <c r="D429" s="3" t="s">
-        <v>944</v>
+        <v>938</v>
       </c>
       <c r="E429" s="18" t="s">
         <v>1677</v>
@@ -19684,21 +19723,21 @@
         <v>1027</v>
       </c>
       <c r="H429" s="3" t="s">
-        <v>942</v>
+        <v>936</v>
       </c>
       <c r="I429" s="3" t="s">
-        <v>942</v>
+        <v>936</v>
       </c>
     </row>
     <row r="430" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A430" s="3" t="s">
-        <v>945</v>
+        <v>939</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>946</v>
+        <v>940</v>
       </c>
       <c r="D430" s="3" t="s">
-        <v>558</v>
+        <v>941</v>
       </c>
       <c r="E430" s="18" t="s">
         <v>1677</v>
@@ -19710,21 +19749,21 @@
         <v>1027</v>
       </c>
       <c r="H430" s="3" t="s">
-        <v>945</v>
+        <v>939</v>
       </c>
       <c r="I430" s="3" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="431" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="431" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A431" s="3" t="s">
-        <v>947</v>
+        <v>942</v>
       </c>
       <c r="B431" s="3" t="s">
-        <v>948</v>
+        <v>943</v>
       </c>
       <c r="D431" s="3" t="s">
-        <v>949</v>
+        <v>944</v>
       </c>
       <c r="E431" s="18" t="s">
         <v>1677</v>
@@ -19736,21 +19775,21 @@
         <v>1027</v>
       </c>
       <c r="H431" s="3" t="s">
-        <v>947</v>
+        <v>942</v>
       </c>
       <c r="I431" s="3" t="s">
-        <v>947</v>
-      </c>
-    </row>
-    <row r="432" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="432" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A432" s="3" t="s">
-        <v>950</v>
+        <v>945</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="D432" s="3" t="s">
-        <v>951</v>
+        <v>558</v>
       </c>
       <c r="E432" s="18" t="s">
         <v>1677</v>
@@ -19762,21 +19801,21 @@
         <v>1027</v>
       </c>
       <c r="H432" s="3" t="s">
-        <v>950</v>
+        <v>945</v>
       </c>
       <c r="I432" s="3" t="s">
-        <v>950</v>
+        <v>945</v>
       </c>
     </row>
     <row r="433" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A433" s="3" t="s">
-        <v>952</v>
+        <v>947</v>
       </c>
       <c r="B433" s="3" t="s">
         <v>948</v>
       </c>
       <c r="D433" s="3" t="s">
-        <v>953</v>
+        <v>949</v>
       </c>
       <c r="E433" s="18" t="s">
         <v>1677</v>
@@ -19788,21 +19827,21 @@
         <v>1027</v>
       </c>
       <c r="H433" s="3" t="s">
-        <v>952</v>
+        <v>947</v>
       </c>
       <c r="I433" s="3" t="s">
-        <v>952</v>
+        <v>947</v>
       </c>
     </row>
     <row r="434" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A434" s="3" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
       <c r="B434" s="3" t="s">
         <v>948</v>
       </c>
       <c r="D434" s="3" t="s">
-        <v>955</v>
+        <v>951</v>
       </c>
       <c r="E434" s="18" t="s">
         <v>1677</v>
@@ -19814,21 +19853,21 @@
         <v>1027</v>
       </c>
       <c r="H434" s="3" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
       <c r="I434" s="3" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
     </row>
     <row r="435" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A435" s="3" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="B435" s="3" t="s">
         <v>948</v>
       </c>
       <c r="D435" s="3" t="s">
-        <v>957</v>
+        <v>953</v>
       </c>
       <c r="E435" s="18" t="s">
         <v>1677</v>
@@ -19840,21 +19879,21 @@
         <v>1027</v>
       </c>
       <c r="H435" s="3" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="I435" s="3" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
     </row>
     <row r="436" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A436" s="3" t="s">
-        <v>958</v>
+        <v>954</v>
       </c>
       <c r="B436" s="3" t="s">
         <v>948</v>
       </c>
       <c r="D436" s="3" t="s">
-        <v>959</v>
+        <v>955</v>
       </c>
       <c r="E436" s="18" t="s">
         <v>1677</v>
@@ -19866,21 +19905,21 @@
         <v>1027</v>
       </c>
       <c r="H436" s="3" t="s">
-        <v>958</v>
+        <v>954</v>
       </c>
       <c r="I436" s="3" t="s">
-        <v>958</v>
-      </c>
-    </row>
-    <row r="437" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A437" s="2" t="s">
-        <v>960</v>
-      </c>
-      <c r="B437" s="2" t="s">
-        <v>961</v>
+        <v>954</v>
+      </c>
+    </row>
+    <row r="437" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A437" s="3" t="s">
+        <v>956</v>
+      </c>
+      <c r="B437" s="3" t="s">
+        <v>948</v>
       </c>
       <c r="D437" s="3" t="s">
-        <v>962</v>
+        <v>957</v>
       </c>
       <c r="E437" s="18" t="s">
         <v>1677</v>
@@ -19891,22 +19930,22 @@
       <c r="G437" s="3" t="s">
         <v>1027</v>
       </c>
-      <c r="H437" s="19" t="s">
-        <v>960</v>
-      </c>
-      <c r="I437" s="2" t="s">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="438" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A438" s="2" t="s">
-        <v>963</v>
-      </c>
-      <c r="B438" s="2" t="s">
-        <v>964</v>
+      <c r="H437" s="3" t="s">
+        <v>956</v>
+      </c>
+      <c r="I437" s="3" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="438" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A438" s="3" t="s">
+        <v>958</v>
+      </c>
+      <c r="B438" s="3" t="s">
+        <v>948</v>
       </c>
       <c r="D438" s="3" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
       <c r="E438" s="18" t="s">
         <v>1677</v>
@@ -19917,19 +19956,19 @@
       <c r="G438" s="3" t="s">
         <v>1027</v>
       </c>
-      <c r="H438" s="19" t="s">
-        <v>963</v>
-      </c>
-      <c r="I438" s="2" t="s">
-        <v>963</v>
+      <c r="H438" s="3" t="s">
+        <v>958</v>
+      </c>
+      <c r="I438" s="3" t="s">
+        <v>958</v>
       </c>
     </row>
     <row r="439" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A439" s="2" t="s">
-        <v>965</v>
+        <v>960</v>
       </c>
       <c r="B439" s="2" t="s">
-        <v>966</v>
+        <v>961</v>
       </c>
       <c r="D439" s="3" t="s">
         <v>962</v>
@@ -19944,18 +19983,18 @@
         <v>1027</v>
       </c>
       <c r="H439" s="19" t="s">
-        <v>965</v>
+        <v>960</v>
       </c>
       <c r="I439" s="2" t="s">
-        <v>965</v>
+        <v>960</v>
       </c>
     </row>
     <row r="440" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A440" s="2" t="s">
-        <v>967</v>
+        <v>963</v>
       </c>
       <c r="B440" s="2" t="s">
-        <v>968</v>
+        <v>964</v>
       </c>
       <c r="D440" s="3" t="s">
         <v>962</v>
@@ -19970,21 +20009,21 @@
         <v>1027</v>
       </c>
       <c r="H440" s="19" t="s">
-        <v>967</v>
+        <v>963</v>
       </c>
       <c r="I440" s="2" t="s">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="441" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="441" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A441" s="2" t="s">
-        <v>969</v>
-      </c>
-      <c r="B441" s="3" t="s">
-        <v>970</v>
+        <v>965</v>
+      </c>
+      <c r="B441" s="2" t="s">
+        <v>966</v>
       </c>
       <c r="D441" s="3" t="s">
-        <v>971</v>
+        <v>962</v>
       </c>
       <c r="E441" s="18" t="s">
         <v>1677</v>
@@ -19996,21 +20035,21 @@
         <v>1027</v>
       </c>
       <c r="H441" s="19" t="s">
-        <v>969</v>
+        <v>965</v>
       </c>
       <c r="I441" s="2" t="s">
-        <v>969</v>
-      </c>
-    </row>
-    <row r="442" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A442" s="3" t="s">
-        <v>972</v>
-      </c>
-      <c r="B442" s="3" t="s">
-        <v>973</v>
+        <v>965</v>
+      </c>
+    </row>
+    <row r="442" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A442" s="2" t="s">
+        <v>967</v>
+      </c>
+      <c r="B442" s="2" t="s">
+        <v>968</v>
       </c>
       <c r="D442" s="3" t="s">
-        <v>974</v>
+        <v>962</v>
       </c>
       <c r="E442" s="18" t="s">
         <v>1677</v>
@@ -20021,22 +20060,22 @@
       <c r="G442" s="3" t="s">
         <v>1027</v>
       </c>
-      <c r="H442" s="3" t="s">
-        <v>972</v>
-      </c>
-      <c r="I442" s="3" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="443" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A443" s="3" t="s">
-        <v>975</v>
+      <c r="H442" s="19" t="s">
+        <v>967</v>
+      </c>
+      <c r="I442" s="2" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="443" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A443" s="2" t="s">
+        <v>969</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>976</v>
+        <v>970</v>
       </c>
       <c r="D443" s="3" t="s">
-        <v>977</v>
+        <v>971</v>
       </c>
       <c r="E443" s="18" t="s">
         <v>1677</v>
@@ -20047,14 +20086,67 @@
       <c r="G443" s="3" t="s">
         <v>1027</v>
       </c>
-      <c r="H443" s="3" t="s">
+      <c r="H443" s="19" t="s">
+        <v>969</v>
+      </c>
+      <c r="I443" s="2" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="444" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A444" s="3" t="s">
+        <v>972</v>
+      </c>
+      <c r="B444" s="3" t="s">
+        <v>973</v>
+      </c>
+      <c r="D444" s="3" t="s">
+        <v>974</v>
+      </c>
+      <c r="E444" s="18" t="s">
+        <v>1677</v>
+      </c>
+      <c r="F444" s="18" t="s">
+        <v>1677</v>
+      </c>
+      <c r="G444" s="3" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H444" s="3" t="s">
+        <v>972</v>
+      </c>
+      <c r="I444" s="3" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="445" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A445" s="3" t="s">
         <v>975</v>
       </c>
-      <c r="I443" s="3" t="s">
+      <c r="B445" s="3" t="s">
+        <v>976</v>
+      </c>
+      <c r="D445" s="3" t="s">
+        <v>977</v>
+      </c>
+      <c r="E445" s="18" t="s">
+        <v>1677</v>
+      </c>
+      <c r="F445" s="18" t="s">
+        <v>1677</v>
+      </c>
+      <c r="G445" s="3" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H445" s="3" t="s">
         <v>975</v>
       </c>
+      <c r="I445" s="3" t="s">
+        <v>975</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J445" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="G2:G1048576">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Inverse">
@@ -20074,7 +20166,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection sqref="A1:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20087,7 +20179,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>1179</v>
+        <v>1736</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>4</v>
@@ -20230,7 +20322,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="C11" t="s">
         <v>991</v>
@@ -20244,7 +20336,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="C12" t="s">
         <v>991</v>

</xml_diff>